<commit_message>
bot sepulveda terminado -v 1.0
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOT CONFRONTACION\Documents\sepulvedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA833326-BB3A-411F-948E-274520D75305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC7A19E-CF69-4038-B66F-C455CCAE4E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29FD356A-5D83-451F-BD5F-77FFF08F5398}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DNI</t>
   </si>
@@ -94,16 +94,30 @@
   </si>
   <si>
     <t>CORRELATIVOS</t>
+  </si>
+  <si>
+    <t>CORREO</t>
+  </si>
+  <si>
+    <t>lcisneros@sempiterno-group.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -146,17 +160,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352DF4CD-3AA4-445E-8DE4-9C2B8C27FA9A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,9 +515,11 @@
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -507,8 +541,11 @@
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -525,9 +562,12 @@
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +582,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -553,7 +593,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -564,7 +604,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -575,7 +615,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -586,7 +626,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -597,7 +637,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -608,7 +648,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -619,7 +659,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -631,7 +671,10 @@
       <c r="G11" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{4E4643D3-2142-42D6-904C-3D849BB8211A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
split in correlative letters
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOT CONFRONTACION\Documents\sepulvedex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\Sepulveda\sepulvedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA833326-BB3A-411F-948E-274520D75305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDBC6E3-CA95-405D-ADF8-B0E8894DC754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29FD356A-5D83-451F-BD5F-77FFF08F5398}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29FD356A-5D83-451F-BD5F-77FFF08F5398}"/>
   </bookViews>
   <sheets>
     <sheet name="conf" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DNI</t>
   </si>
@@ -75,9 +75,6 @@
     <t>SEXT</t>
   </si>
   <si>
-    <t>SETIM</t>
-  </si>
-  <si>
     <t>OCTAV</t>
   </si>
   <si>
@@ -94,6 +91,15 @@
   </si>
   <si>
     <t>CORRELATIVOS</t>
+  </si>
+  <si>
+    <t>DOCUMENTO NACIONAL DE IDENTIDAD N°</t>
+  </si>
+  <si>
+    <t>PREFIJO CORRELATIVO</t>
+  </si>
+  <si>
+    <t>SETIM,SÉPTIM</t>
   </si>
 </sst>
 </file>
@@ -150,11 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352DF4CD-3AA4-445E-8DE4-9C2B8C27FA9A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +490,7 @@
     <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -496,19 +501,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -518,7 +526,7 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
@@ -527,13 +535,13 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
@@ -542,90 +550,92 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>

</xml_diff>

<commit_message>
working on sending emails
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\Sepulveda\sepulvedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDBC6E3-CA95-405D-ADF8-B0E8894DC754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19593AAD-BF72-4EA4-B7F8-31F14763B8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29FD356A-5D83-451F-BD5F-77FFF08F5398}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>DNI</t>
   </si>
@@ -57,33 +57,12 @@
     <t>SOMBREAR</t>
   </si>
   <si>
-    <t>PRIMER</t>
-  </si>
-  <si>
-    <t>SEGUND</t>
-  </si>
-  <si>
-    <t>TERCER</t>
-  </si>
-  <si>
-    <t>CUART</t>
-  </si>
-  <si>
-    <t>QUINT</t>
-  </si>
-  <si>
-    <t>SEXT</t>
-  </si>
-  <si>
     <t>OCTAV</t>
   </si>
   <si>
     <t>NOVEN</t>
   </si>
   <si>
-    <t>DECIM</t>
-  </si>
-  <si>
     <t>CE</t>
   </si>
   <si>
@@ -99,7 +78,58 @@
     <t>PREFIJO CORRELATIVO</t>
   </si>
   <si>
-    <t>SETIM,SÉPTIM</t>
+    <t>SETIM,SÉPTIM,SÉTIM</t>
+  </si>
+  <si>
+    <t>DECIM,DÉCIM</t>
+  </si>
+  <si>
+    <t>DÉCIMO SEGUND</t>
+  </si>
+  <si>
+    <t>DÉCIMO TERCER</t>
+  </si>
+  <si>
+    <t>DÉCIMO CUART</t>
+  </si>
+  <si>
+    <t>DÉCIMO QUINT</t>
+  </si>
+  <si>
+    <t>DÉCIMO SEXT</t>
+  </si>
+  <si>
+    <t>DÉCIMO SÉTIM</t>
+  </si>
+  <si>
+    <t>DÉCIM OCTAV</t>
+  </si>
+  <si>
+    <t>DÉCIM NOVEN</t>
+  </si>
+  <si>
+    <t>VIGÉSIM</t>
+  </si>
+  <si>
+    <t>QUINT,CLAUSULA QUINT</t>
+  </si>
+  <si>
+    <t>SEXT,CLAUSULA SEXT</t>
+  </si>
+  <si>
+    <t>PRIMER,CLAUSULA PRIMER</t>
+  </si>
+  <si>
+    <t>SEGUND,CLAUSULA SEGUND</t>
+  </si>
+  <si>
+    <t>TERCER,CLAUSULA TERCER</t>
+  </si>
+  <si>
+    <t>CUART,CLAUSULA CUART</t>
+  </si>
+  <si>
+    <t>DÉCIMO PRIMER,DÉCIMA PRIMER</t>
   </si>
 </sst>
 </file>
@@ -129,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,14 +182,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,20 +516,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352DF4CD-3AA4-445E-8DE4-9C2B8C27FA9A}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -501,19 +544,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -528,7 +571,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -543,7 +586,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>8</v>
@@ -552,13 +595,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -569,7 +612,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -580,7 +623,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -591,7 +634,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -602,7 +645,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -613,7 +656,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -624,7 +667,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -640,6 +683,56 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>